<commit_message>
remove duplicate rows, add reports not in cases There should not be any more duplicate rows in any of the output files. "output files/incident numbers that didn't reach DA.xlsx" contains all the police report data with incident numbers not in the District_Attorney_Incoming_Caseload file.
</commit_message>
<xml_diff>
--- a/output files/Arson BY YEAR.xlsx
+++ b/output files/Arson BY YEAR.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,6 +35,9 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -44,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -67,16 +70,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,139 +526,139 @@
   </sheetPr>
   <dimension ref="A1:Z131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>index</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Incident Number</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Incident Date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Incident Category</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Incident Subcategory</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Incident Description</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Incident Code</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Court Number</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Filed.Charge.List</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Arrest Date</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Filing Date</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>Dispo Code</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Dispo Description</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>Dispo Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>Outcome Sub-Type Description</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>Dispo Case Type</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>Sentence Type</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>SP Term</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>CJ Term</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>Supervision Term</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>Forfeiture</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>Outcome Description</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>dismissed</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>ordering</t>
         </is>
@@ -15073,7 +15085,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
@@ -15095,132 +15107,132 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>index</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Incident Number</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Incident Date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Incident Category</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Incident Subcategory</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Incident Description</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Incident Code</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Court Number</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Filed.Charge.List</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Arrest Date</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Filing Date</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>Dispo Code</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Dispo Description</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>Dispo Date</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>Outcome Sub-Type Description</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>Dispo Case Type</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>Sentence Type</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>SP Term</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>CJ Term</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>Supervision Term</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>Forfeiture</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>Outcome Description</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>dismissed</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>ordering</t>
         </is>
@@ -27135,7 +27147,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>

</xml_diff>